<commit_message>
Add second way to calculate estimateWinner endpoint, add addContracts endpoint
</commit_message>
<xml_diff>
--- a/files/input/companiesDataMDB.xlsx
+++ b/files/input/companiesDataMDB.xlsx
@@ -19,20 +19,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="54">
   <si>
     <t>minVolume</t>
   </si>
   <si>
-    <t>JONESBORO SPÓŁKA Z OGRANICZONĄ ODPOWIEDZIALNOŚCIĄ</t>
-  </si>
-  <si>
-    <t>"KODREWEX" SPÓŁKA Z OGRANICZONĄ ODPOWIEDZIALNOŚCIĄ</t>
-  </si>
-  <si>
-    <t>PALOMINO Justyna Jaskulska</t>
-  </si>
-  <si>
     <t>isLegalPerson</t>
   </si>
   <si>
@@ -139,6 +130,57 @@
   </si>
   <si>
     <t>345678912</t>
+  </si>
+  <si>
+    <t>1111111111</t>
+  </si>
+  <si>
+    <t>2222222222</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>aa</t>
+  </si>
+  <si>
+    <t>aaa</t>
+  </si>
+  <si>
+    <t>aaaa</t>
+  </si>
+  <si>
+    <t>aaaaa</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>bb</t>
+  </si>
+  <si>
+    <t>bbb</t>
+  </si>
+  <si>
+    <t>bbbbb</t>
+  </si>
+  <si>
+    <t>bbbb</t>
   </si>
 </sst>
 </file>
@@ -459,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,40 +522,40 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B1" t="s">
+      <c r="G1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C1" t="s">
+      <c r="H1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D1" t="s">
+      <c r="I1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
       <c r="K1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="M1" t="s">
         <v>0</v>
@@ -521,68 +563,68 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="H2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="J2" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2">
-        <v>5</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="I3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="L3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="M3">
         <v>5</v>
@@ -590,41 +632,117 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="H4" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4">
-        <v>5</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="M5">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I6" t="s">
+        <v>52</v>
+      </c>
+      <c r="J6" t="s">
+        <v>53</v>
+      </c>
+      <c r="K6" t="s">
+        <v>30</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add generateContractNumber util function, add it to addContracts endpoint
</commit_message>
<xml_diff>
--- a/files/input/companiesDataMDB.xlsx
+++ b/files/input/companiesDataMDB.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="66">
   <si>
     <t>minVolume</t>
   </si>
@@ -138,12 +138,6 @@
     <t>2222222222</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
     <t>Z</t>
   </si>
   <si>
@@ -217,6 +211,12 @@
   </si>
   <si>
     <t>dddd</t>
+  </si>
+  <si>
+    <t>P.P.H.U. "Asdasdad "asda a-123!#!@*@o%!@)#)</t>
+  </si>
+  <si>
+    <t>P.P.H.U. "=-1239309427//..,.;'SDF,ŻĄŁÓQMOPEJWQ`` SDF DFADF asfldf hdas alksdjfha asdklfjas dfasfjk aslkjdf asldfk</t>
   </si>
 </sst>
 </file>
@@ -540,7 +540,7 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,7 +602,7 @@
         <v>31</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
@@ -628,7 +628,9 @@
       <c r="J2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="1"/>
+      <c r="K2" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="L2" s="1"/>
       <c r="M2">
         <v>4.5</v>
@@ -638,8 +640,8 @@
       <c r="A3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B3" t="s">
-        <v>40</v>
+      <c r="B3" s="1" t="s">
+        <v>65</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -671,7 +673,7 @@
         <v>33</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>8</v>
@@ -710,31 +712,31 @@
         <v>37</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="F5" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="G5" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="H5" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K5" s="3" t="s">
         <v>30</v>
@@ -748,31 +750,31 @@
         <v>38</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" t="s">
         <v>49</v>
       </c>
-      <c r="D6" t="s">
+      <c r="F6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E6" t="s">
+      <c r="H6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I6" t="s">
+        <v>50</v>
+      </c>
+      <c r="J6" t="s">
         <v>51</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I6" t="s">
-        <v>52</v>
-      </c>
-      <c r="J6" t="s">
-        <v>53</v>
       </c>
       <c r="K6" t="s">
         <v>30</v>
@@ -783,34 +785,34 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="D7" t="s">
         <v>55</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7" t="s">
         <v>56</v>
       </c>
-      <c r="D7" t="s">
+      <c r="F7" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E7" t="s">
-        <v>58</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="G7" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K7" t="s">
         <v>30</v>
@@ -821,34 +823,34 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" t="s">
         <v>60</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="D8" t="s">
         <v>61</v>
       </c>
-      <c r="C8" t="s">
+      <c r="E8" t="s">
         <v>62</v>
       </c>
-      <c r="D8" t="s">
+      <c r="F8" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E8" t="s">
-        <v>64</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="G8" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L8" t="s">
         <v>30</v>

</xml_diff>